<commit_message>
pgd not working for reactive!?
</commit_message>
<xml_diff>
--- a/Initial presentation/Codi/PGD/data_10PQ.xlsx
+++ b/Initial presentation/Codi/PGD/data_10PQ.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\Desktop\CITCEA\Codi\PGD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\CITCEA\Initial presentation\Codi\PGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18908D19-6BBA-4939-8D12-3196077D2D78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43544277-89E4-4F72-87F2-FECA9F9384A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
     <sheet name="lines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,14 +426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A9F03E-3FB2-47D9-B81B-D17612DC601D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -734,8 +733,7 @@
         <v>-0.1</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -764,7 +762,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -789,14 +787,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAEDE02B-082B-43FE-958E-56326AECD5D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1106,8 +1104,7 @@
         <v>0.01</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -1140,7 +1137,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
debug PGD chart dataframe
</commit_message>
<xml_diff>
--- a/Initial presentation/Codi/PGD/data_10PQ.xlsx
+++ b/Initial presentation/Codi/PGD/data_10PQ.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\CITCEA\Initial presentation\Codi\PGD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\Desktop\CITCEA\Initial presentation\Codi\PGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C215109D-B1A5-478F-BD6D-D466C27228C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28815" yWindow="60" windowWidth="10860" windowHeight="8925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
     <sheet name="lines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,14 +428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -733,7 +735,7 @@
         <v>-0.1</v>
       </c>
       <c r="C12">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -762,7 +764,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -787,14 +789,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1104,7 +1106,7 @@
         <v>0.01</v>
       </c>
       <c r="D11">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -1135,9 +1137,9 @@
       <c r="C12">
         <v>0.01</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>

</xml_diff>